<commit_message>
dados da planilha inseridos no banco de dados
</commit_message>
<xml_diff>
--- a/extras_files/criacao_registros/crismandos_ficticios.xlsx
+++ b/extras_files/criacao_registros/crismandos_ficticios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MeusRepositorios\frequencia.simples\extras_files\criacao_registros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70CE6EB9-7625-4598-BA23-0C26A04EAA69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E993D6F-7166-4C20-B6DE-E032A53B3012}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,42 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="378">
   <si>
-    <t>Nome</t>
-  </si>
-  <si>
-    <t>Nome da Mãe</t>
-  </si>
-  <si>
-    <t>Nome do Pai</t>
-  </si>
-  <si>
-    <t>Data de Nascimento</t>
-  </si>
-  <si>
-    <t>Endereço</t>
-  </si>
-  <si>
-    <t>Cidade</t>
-  </si>
-  <si>
-    <t>Telefone 1</t>
-  </si>
-  <si>
-    <t>Telefone 2</t>
-  </si>
-  <si>
-    <t>Recebeu Eucaristia</t>
-  </si>
-  <si>
-    <t>Recebeu Batismo</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>ID Catequista</t>
-  </si>
-  <si>
     <t>João Guilherme Jesus</t>
   </si>
   <si>
@@ -1154,6 +1118,42 @@
   </si>
   <si>
     <t>+55 (061) 9807 2137</t>
+  </si>
+  <si>
+    <t>nome</t>
+  </si>
+  <si>
+    <t>nome_mae</t>
+  </si>
+  <si>
+    <t>nome_pai</t>
+  </si>
+  <si>
+    <t>data_nascimento</t>
+  </si>
+  <si>
+    <t>endereco</t>
+  </si>
+  <si>
+    <t>cidade</t>
+  </si>
+  <si>
+    <t>tel1</t>
+  </si>
+  <si>
+    <t>tel2</t>
+  </si>
+  <si>
+    <t>eucaristia</t>
+  </si>
+  <si>
+    <t>batismo</t>
+  </si>
+  <si>
+    <t>status_crismando</t>
+  </si>
+  <si>
+    <t>fk_id_catequista</t>
   </si>
 </sst>
 </file>
@@ -1518,8 +1518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B29" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1533,81 +1533,81 @@
     <col min="7" max="8" width="17.88671875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.77734375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>366</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>367</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>368</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>369</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>370</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>371</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>372</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>373</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>374</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>9</v>
+        <v>375</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>10</v>
+        <v>376</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>11</v>
+        <v>377</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="G2" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="H2" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="I2" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="J2" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="K2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="L2">
         <v>2</v>
@@ -1615,37 +1615,37 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="G3" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="H3" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="I3" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="J3" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="K3" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="L3">
         <v>1</v>
@@ -1653,34 +1653,34 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="F4" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="G4" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="I4" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="J4" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="K4" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="L4">
         <v>2</v>
@@ -1688,34 +1688,34 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="E5" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="F5" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="G5" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="I5" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="J5" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="K5" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="L5">
         <v>1</v>
@@ -1723,37 +1723,37 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="E6" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="F6" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="H6" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="I6" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="J6" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="K6" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="L6">
         <v>2</v>
@@ -1761,34 +1761,34 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D7" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="E7" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="F7" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="G7" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="I7" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="J7" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="K7" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="L7">
         <v>1</v>
@@ -1796,34 +1796,34 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="B8" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C8" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="D8" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="E8" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F8" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="G8" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="I8" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="J8" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="K8" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="L8">
         <v>2</v>
@@ -1831,37 +1831,37 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="C9" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="D9" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="E9" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="F9" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="G9" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="H9" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="I9" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="J9" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="K9" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="L9">
         <v>1</v>
@@ -1869,37 +1869,37 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="B10" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="C10" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D10" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="E10" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="F10" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="G10" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="H10" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="I10" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="J10" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="K10" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="L10">
         <v>2</v>
@@ -1907,34 +1907,34 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="B11" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="C11" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="D11" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="E11" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="F11" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="G11" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="I11" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="J11" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="K11" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="L11">
         <v>1</v>
@@ -1942,34 +1942,34 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B12" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="C12" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="D12" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="E12" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="F12" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="G12" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="I12" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="J12" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="K12" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="L12">
         <v>1</v>
@@ -1977,34 +1977,34 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B13" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="C13" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="D13" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="E13" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="F13" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="G13" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="I13" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="J13" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="K13" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="L13">
         <v>1</v>
@@ -2012,34 +2012,34 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="B14" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="C14" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="D14" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="E14" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="F14" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="G14" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="I14" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="J14" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="K14" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="L14">
         <v>2</v>
@@ -2047,34 +2047,34 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="B15" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="C15" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="D15" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="E15" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="F15" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="G15" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="I15" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="J15" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="K15" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="L15">
         <v>2</v>
@@ -2082,37 +2082,37 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="B16" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="C16" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="D16" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E16" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F16" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="G16" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="H16" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="I16" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="J16" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="K16" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="L16">
         <v>1</v>
@@ -2120,34 +2120,34 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="B17" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="C17" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="D17" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="E17" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="F17" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="G17" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="I17" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="J17" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="K17" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="L17">
         <v>2</v>
@@ -2155,37 +2155,37 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="B18" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="C18" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="D18" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="E18" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="F18" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="G18" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="H18" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="I18" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="J18" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="K18" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="L18">
         <v>1</v>
@@ -2193,37 +2193,37 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="B19" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="C19" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="D19" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="E19" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="F19" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="G19" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="H19" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="I19" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="J19" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="K19" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="L19">
         <v>2</v>
@@ -2231,37 +2231,37 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="B20" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="C20" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="D20" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="E20" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="F20" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="G20" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="H20" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="I20" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="J20" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="K20" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="L20">
         <v>2</v>
@@ -2269,34 +2269,34 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="B21" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="C21" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="D21" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="E21" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="F21" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="G21" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="I21" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="J21" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="K21" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="L21">
         <v>2</v>
@@ -2304,34 +2304,34 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="B22" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="C22" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="D22" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="E22" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="F22" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="G22" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="I22" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="J22" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="K22" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="L22">
         <v>2</v>
@@ -2339,37 +2339,37 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="B23" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="C23" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="D23" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="E23" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="F23" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="G23" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="H23" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="I23" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="J23" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="K23" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="L23">
         <v>2</v>
@@ -2377,34 +2377,34 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="B24" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="C24" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="D24" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="E24" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="F24" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="G24" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="I24" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="J24" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="K24" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="L24">
         <v>1</v>
@@ -2412,37 +2412,37 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="B25" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="C25" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="D25" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="E25" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="F25" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="G25" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="H25" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="I25" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="J25" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="K25" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="L25">
         <v>2</v>
@@ -2450,34 +2450,34 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="B26" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="C26" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="D26" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="E26" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="F26" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="G26" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="I26" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="J26" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="K26" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="L26">
         <v>1</v>
@@ -2485,37 +2485,37 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="B27" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="C27" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="D27" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="E27" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="F27" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="G27" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="H27" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="I27" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="J27" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="K27" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="L27">
         <v>2</v>
@@ -2523,37 +2523,37 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="B28" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="C28" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="D28" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="E28" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="F28" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="G28" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="H28" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="I28" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="J28" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="K28" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="L28">
         <v>1</v>
@@ -2561,34 +2561,34 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="B29" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="C29" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="D29" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="E29" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="F29" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="G29" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="I29" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="J29" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="K29" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="L29">
         <v>2</v>
@@ -2596,37 +2596,37 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="B30" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="C30" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="D30" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="E30" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="F30" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="G30" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="H30" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="I30" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="J30" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="K30" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="L30">
         <v>1</v>
@@ -2634,37 +2634,37 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="B31" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="C31" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="D31" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="E31" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="F31" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="G31" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="H31" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="I31" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="J31" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="K31" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="L31">
         <v>2</v>
@@ -2672,37 +2672,37 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="B32" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="C32" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="D32" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="E32" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="F32" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="G32" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="H32" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="I32" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="J32" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="K32" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="L32">
         <v>2</v>
@@ -2710,34 +2710,34 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="B33" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="C33" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="D33" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="E33" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="F33" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="G33" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="I33" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="J33" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="K33" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="L33">
         <v>2</v>
@@ -2745,34 +2745,34 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="B34" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="C34" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="D34" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="E34" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="F34" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="G34" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="I34" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="J34" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="K34" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="L34">
         <v>1</v>
@@ -2780,37 +2780,37 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="B35" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="C35" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="D35" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="E35" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="F35" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="G35" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="H35" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="I35" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="J35" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="K35" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="L35">
         <v>1</v>
@@ -2818,34 +2818,34 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="B36" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="C36" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
       <c r="D36" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="E36" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="F36" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="G36" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
       <c r="I36" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="J36" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="K36" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="L36">
         <v>2</v>
@@ -2853,37 +2853,37 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="B37" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="C37" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="D37" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="E37" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="F37" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="G37" t="s">
-        <v>251</v>
+        <v>239</v>
       </c>
       <c r="H37" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="I37" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="J37" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="K37" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="L37">
         <v>2</v>
@@ -2891,37 +2891,37 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="B38" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
       <c r="C38" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="D38" t="s">
-        <v>256</v>
+        <v>244</v>
       </c>
       <c r="E38" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
       <c r="F38" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="G38" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
       <c r="H38" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="I38" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="J38" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="K38" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="L38">
         <v>2</v>
@@ -2929,37 +2929,37 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
       <c r="B39" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
       <c r="C39" t="s">
-        <v>262</v>
+        <v>250</v>
       </c>
       <c r="D39" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
       <c r="E39" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
       <c r="F39" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="G39" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
       <c r="H39" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="I39" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="J39" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="K39" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="L39">
         <v>1</v>
@@ -2967,34 +2967,34 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="B40" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="C40" t="s">
-        <v>269</v>
+        <v>257</v>
       </c>
       <c r="D40" t="s">
-        <v>270</v>
+        <v>258</v>
       </c>
       <c r="E40" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
       <c r="F40" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="G40" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
       <c r="I40" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="J40" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="K40" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="L40">
         <v>2</v>
@@ -3002,34 +3002,34 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="B41" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="C41" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
       <c r="D41" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
       <c r="E41" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
       <c r="F41" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="G41" t="s">
-        <v>278</v>
+        <v>266</v>
       </c>
       <c r="I41" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="J41" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="K41" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="L41">
         <v>2</v>
@@ -3037,34 +3037,34 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>279</v>
+        <v>267</v>
       </c>
       <c r="B42" t="s">
-        <v>280</v>
+        <v>268</v>
       </c>
       <c r="C42" t="s">
-        <v>281</v>
+        <v>269</v>
       </c>
       <c r="D42" t="s">
-        <v>282</v>
+        <v>270</v>
       </c>
       <c r="E42" t="s">
-        <v>283</v>
+        <v>271</v>
       </c>
       <c r="F42" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="G42" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
       <c r="I42" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="J42" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="K42" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="L42">
         <v>1</v>
@@ -3072,34 +3072,34 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>285</v>
+        <v>273</v>
       </c>
       <c r="B43" t="s">
-        <v>286</v>
+        <v>274</v>
       </c>
       <c r="C43" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
       <c r="D43" t="s">
-        <v>288</v>
+        <v>276</v>
       </c>
       <c r="E43" t="s">
-        <v>289</v>
+        <v>277</v>
       </c>
       <c r="F43" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="G43" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="I43" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="J43" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="K43" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="L43">
         <v>2</v>
@@ -3107,34 +3107,34 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>291</v>
+        <v>279</v>
       </c>
       <c r="B44" t="s">
-        <v>292</v>
+        <v>280</v>
       </c>
       <c r="C44" t="s">
-        <v>293</v>
+        <v>281</v>
       </c>
       <c r="D44" t="s">
-        <v>294</v>
+        <v>282</v>
       </c>
       <c r="E44" t="s">
-        <v>295</v>
+        <v>283</v>
       </c>
       <c r="F44" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="G44" t="s">
-        <v>296</v>
+        <v>284</v>
       </c>
       <c r="I44" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="J44" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="K44" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="L44">
         <v>1</v>
@@ -3142,34 +3142,34 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>297</v>
+        <v>285</v>
       </c>
       <c r="B45" t="s">
-        <v>298</v>
+        <v>286</v>
       </c>
       <c r="C45" t="s">
-        <v>299</v>
+        <v>287</v>
       </c>
       <c r="D45" t="s">
-        <v>300</v>
+        <v>288</v>
       </c>
       <c r="E45" t="s">
-        <v>301</v>
+        <v>289</v>
       </c>
       <c r="F45" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="G45" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
       <c r="I45" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="J45" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="K45" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="L45">
         <v>1</v>
@@ -3177,37 +3177,37 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>303</v>
+        <v>291</v>
       </c>
       <c r="B46" t="s">
-        <v>304</v>
+        <v>292</v>
       </c>
       <c r="C46" t="s">
-        <v>305</v>
+        <v>293</v>
       </c>
       <c r="D46" t="s">
-        <v>306</v>
+        <v>294</v>
       </c>
       <c r="E46" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="F46" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="G46" t="s">
-        <v>308</v>
+        <v>296</v>
       </c>
       <c r="H46" t="s">
-        <v>309</v>
+        <v>297</v>
       </c>
       <c r="I46" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="J46" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="K46" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="L46">
         <v>1</v>
@@ -3215,37 +3215,37 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>310</v>
+        <v>298</v>
       </c>
       <c r="B47" t="s">
-        <v>311</v>
+        <v>299</v>
       </c>
       <c r="C47" t="s">
-        <v>312</v>
+        <v>300</v>
       </c>
       <c r="D47" t="s">
-        <v>313</v>
+        <v>301</v>
       </c>
       <c r="E47" t="s">
-        <v>314</v>
+        <v>302</v>
       </c>
       <c r="F47" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="G47" t="s">
-        <v>315</v>
+        <v>303</v>
       </c>
       <c r="H47" t="s">
-        <v>316</v>
+        <v>304</v>
       </c>
       <c r="I47" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="J47" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="K47" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="L47">
         <v>2</v>
@@ -3253,37 +3253,37 @@
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>317</v>
+        <v>305</v>
       </c>
       <c r="B48" t="s">
-        <v>318</v>
+        <v>306</v>
       </c>
       <c r="C48" t="s">
-        <v>319</v>
+        <v>307</v>
       </c>
       <c r="D48" t="s">
-        <v>320</v>
+        <v>308</v>
       </c>
       <c r="E48" t="s">
-        <v>321</v>
+        <v>309</v>
       </c>
       <c r="F48" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="G48" t="s">
-        <v>322</v>
+        <v>310</v>
       </c>
       <c r="H48" t="s">
-        <v>323</v>
+        <v>311</v>
       </c>
       <c r="I48" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="J48" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="K48" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="L48">
         <v>1</v>
@@ -3291,37 +3291,37 @@
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>324</v>
+        <v>312</v>
       </c>
       <c r="B49" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
       <c r="C49" t="s">
-        <v>326</v>
+        <v>314</v>
       </c>
       <c r="D49" t="s">
-        <v>327</v>
+        <v>315</v>
       </c>
       <c r="E49" t="s">
-        <v>328</v>
+        <v>316</v>
       </c>
       <c r="F49" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="G49" t="s">
-        <v>329</v>
+        <v>317</v>
       </c>
       <c r="H49" t="s">
-        <v>330</v>
+        <v>318</v>
       </c>
       <c r="I49" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="J49" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="K49" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="L49">
         <v>1</v>
@@ -3329,37 +3329,37 @@
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>331</v>
+        <v>319</v>
       </c>
       <c r="B50" t="s">
-        <v>332</v>
+        <v>320</v>
       </c>
       <c r="C50" t="s">
-        <v>333</v>
+        <v>321</v>
       </c>
       <c r="D50" t="s">
-        <v>334</v>
+        <v>322</v>
       </c>
       <c r="E50" t="s">
-        <v>335</v>
+        <v>323</v>
       </c>
       <c r="F50" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="G50" t="s">
-        <v>336</v>
+        <v>324</v>
       </c>
       <c r="H50" t="s">
-        <v>337</v>
+        <v>325</v>
       </c>
       <c r="I50" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="J50" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="K50" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="L50">
         <v>2</v>
@@ -3367,37 +3367,37 @@
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>338</v>
+        <v>326</v>
       </c>
       <c r="B51" t="s">
-        <v>339</v>
+        <v>327</v>
       </c>
       <c r="C51" t="s">
-        <v>340</v>
+        <v>328</v>
       </c>
       <c r="D51" t="s">
-        <v>341</v>
+        <v>329</v>
       </c>
       <c r="E51" t="s">
-        <v>342</v>
+        <v>330</v>
       </c>
       <c r="F51" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="G51" t="s">
-        <v>343</v>
+        <v>331</v>
       </c>
       <c r="H51" t="s">
-        <v>344</v>
+        <v>332</v>
       </c>
       <c r="I51" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="J51" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="K51" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="L51">
         <v>1</v>
@@ -3405,37 +3405,37 @@
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>345</v>
+        <v>333</v>
       </c>
       <c r="B52" t="s">
-        <v>346</v>
+        <v>334</v>
       </c>
       <c r="C52" t="s">
-        <v>347</v>
+        <v>335</v>
       </c>
       <c r="D52" t="s">
-        <v>348</v>
+        <v>336</v>
       </c>
       <c r="E52" t="s">
-        <v>349</v>
+        <v>337</v>
       </c>
       <c r="F52" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="G52" t="s">
-        <v>350</v>
+        <v>338</v>
       </c>
       <c r="H52" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="I52" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="J52" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="K52" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="L52">
         <v>2</v>
@@ -3443,37 +3443,37 @@
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>352</v>
+        <v>340</v>
       </c>
       <c r="B53" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="C53" t="s">
-        <v>354</v>
+        <v>342</v>
       </c>
       <c r="D53" t="s">
-        <v>355</v>
+        <v>343</v>
       </c>
       <c r="E53" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="F53" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="G53" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="H53" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="I53" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="J53" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="K53" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="L53">
         <v>2</v>
@@ -3481,34 +3481,34 @@
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>359</v>
+        <v>347</v>
       </c>
       <c r="B54" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="C54" t="s">
-        <v>361</v>
+        <v>349</v>
       </c>
       <c r="D54" t="s">
-        <v>362</v>
+        <v>350</v>
       </c>
       <c r="E54" t="s">
-        <v>363</v>
+        <v>351</v>
       </c>
       <c r="F54" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="G54" t="s">
-        <v>364</v>
+        <v>352</v>
       </c>
       <c r="I54" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="J54" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="K54" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="L54">
         <v>1</v>
@@ -3516,34 +3516,34 @@
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>365</v>
+        <v>353</v>
       </c>
       <c r="B55" t="s">
-        <v>366</v>
+        <v>354</v>
       </c>
       <c r="C55" t="s">
-        <v>367</v>
+        <v>355</v>
       </c>
       <c r="D55" t="s">
-        <v>368</v>
+        <v>356</v>
       </c>
       <c r="E55" t="s">
-        <v>369</v>
+        <v>357</v>
       </c>
       <c r="F55" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="G55" t="s">
-        <v>370</v>
+        <v>358</v>
       </c>
       <c r="I55" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="J55" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="K55" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="L55">
         <v>2</v>
@@ -3551,37 +3551,37 @@
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>371</v>
+        <v>359</v>
       </c>
       <c r="B56" t="s">
-        <v>372</v>
+        <v>360</v>
       </c>
       <c r="C56" t="s">
-        <v>373</v>
+        <v>361</v>
       </c>
       <c r="D56" t="s">
-        <v>374</v>
+        <v>362</v>
       </c>
       <c r="E56" t="s">
-        <v>375</v>
+        <v>363</v>
       </c>
       <c r="F56" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="G56" t="s">
-        <v>376</v>
+        <v>364</v>
       </c>
       <c r="H56" t="s">
-        <v>377</v>
+        <v>365</v>
       </c>
       <c r="I56" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="J56" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="K56" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="L56">
         <v>1</v>

</xml_diff>